<commit_message>
-Added 5V Regulator Circuit to Schematic -Added Crystal Oscillator Part to Schematic -Updated BOM with new parts -Added footprints for Capacitors C1, C2
</commit_message>
<xml_diff>
--- a/Modular Circuit Board/Z80 Modular Circuit Board - BOM.xlsx
+++ b/Modular Circuit Board/Z80 Modular Circuit Board - BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Product Name</t>
   </si>
@@ -69,6 +69,54 @@
   </si>
   <si>
     <t>MC7805ABD2TG</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Nichicon 0.33uF Electrolytic Capacitor</t>
+  </si>
+  <si>
+    <t>0.33uF 50V 4mm Radial Through Hole</t>
+  </si>
+  <si>
+    <t>475-8983</t>
+  </si>
+  <si>
+    <t>USR1HR33MDD</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Nichicon 1uF Electrolytic Capacitor</t>
+  </si>
+  <si>
+    <t>1uF 50V 5mm Radial Through Hole</t>
+  </si>
+  <si>
+    <t>715-2808</t>
+  </si>
+  <si>
+    <t>UPW1H010MDD</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>Mercury 4MHz Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>4MHz +-50ppm HCMOS TTL Crystal Oscillator</t>
+  </si>
+  <si>
+    <t>767-5244</t>
+  </si>
+  <si>
+    <t>5H14ET-4.000</t>
+  </si>
+  <si>
+    <t>O1</t>
   </si>
 </sst>
 </file>
@@ -155,13 +203,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -482,7 +530,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,44 +540,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -543,10 +591,10 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>C3*D3</f>
         <v>0.57999999999999996</v>
       </c>
@@ -559,56 +607,106 @@
       <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E4" s="3">
         <f t="shared" ref="E4:E15" si="0">C4*D4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+        <v>0.38</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.111</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.81</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>1.81</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -621,8 +719,8 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -635,8 +733,8 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -649,8 +747,8 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -663,8 +761,8 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -677,8 +775,8 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -691,8 +789,8 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -705,8 +803,8 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -719,8 +817,8 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>